<commit_message>
Mapeamento de tipos de dados
</commit_message>
<xml_diff>
--- a/modelagem/business_matrix.xlsx
+++ b/modelagem/business_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\analise-dados-evasao\modelagem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F23078-BE24-4639-B7E2-A2E064444FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45905DF5-4184-4551-93D3-034AA579093A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1329,7 +1329,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>